<commit_message>
Weekly homework and data exploration with my data set.
</commit_message>
<xml_diff>
--- a/project/tidydata/foodconsumptionRdata.xlsx
+++ b/project/tidydata/foodconsumptionRdata.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiffa\OneDrive\Documents\2019 Fall Courses ISU\590A R\Repository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiffa\OneDrive\Documents\R\Repository\project\tidydata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52A2E2B-6D78-4420-89CB-5539DE35D3C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E6B6FB-9833-4FF2-9AB1-73A04D17FE10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A707520-144D-48CE-A482-07B2D71A8EBC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Food Consumption By Category" sheetId="1" r:id="rId1"/>
+    <sheet name="Vegetable Fruit and Grain Cons" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="74">
   <si>
     <t>lowus</t>
   </si>
@@ -126,6 +127,135 @@
   </si>
   <si>
     <t>uphincome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Apples, Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Apples as fruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Apple juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Bananas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Berries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Grapes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Melons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Oranges, Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Oranges as fruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Orange juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Other citrus fruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Stone fruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Tropical fruit</t>
+  </si>
+  <si>
+    <t>Vegetables, Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Brassica, Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Broccoli and cauliflower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Carrots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Celery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Cucumbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Green Peas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Leafy vegetable, Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Lettuce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Onions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Peppers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Tomatoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Sweet corn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Potatoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Snap beans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Legumes dried</t>
+  </si>
+  <si>
+    <t>Fruit Total</t>
+  </si>
+  <si>
+    <t>Grains, Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Corn flour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Oat flour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Rice dried</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Wheat flour</t>
+  </si>
+  <si>
+    <t>Nuts, Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Peanuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Tree nuts</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>95% CI</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Upper</t>
   </si>
 </sst>
 </file>
@@ -155,7 +285,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -163,14 +293,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +685,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4922D271-3482-4991-9771-EF98DCE33823}">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
@@ -506,7 +706,7 @@
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -529,7 +729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -567,7 +767,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -605,7 +805,7 @@
         <v>115.69</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -643,7 +843,7 @@
         <v>113.4221</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -681,7 +881,7 @@
         <v>180.35</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -719,7 +919,7 @@
         <v>86.65</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -757,7 +957,7 @@
         <v>96.52</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -795,7 +995,7 @@
         <v>29.38</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -832,8 +1032,9 @@
       <c r="L9" s="1">
         <v>19.18</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -871,7 +1072,7 @@
         <v>68.608100000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -909,7 +1110,7 @@
         <v>46.3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -947,7 +1148,7 @@
         <v>57.04</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -985,7 +1186,7 @@
         <v>41.9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1023,7 +1224,7 @@
         <v>20.49</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1262,7 @@
         <v>109.54</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2397,4 +2598,574 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF0BA0-5ABF-4BCB-AFC2-6FFDB4FE4139}">
+  <dimension ref="A1:D40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <v>108.55</v>
+      </c>
+      <c r="C3" s="1">
+        <v>107.6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>109.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1">
+        <v>24.59</v>
+      </c>
+      <c r="C4" s="1">
+        <v>24.24</v>
+      </c>
+      <c r="D4" s="1">
+        <v>24.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1">
+        <v>13.27</v>
+      </c>
+      <c r="C5" s="1">
+        <v>13.07</v>
+      </c>
+      <c r="D5" s="1">
+        <v>13.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1">
+        <v>11.11</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10.83</v>
+      </c>
+      <c r="D6" s="1">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10.44</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10.31</v>
+      </c>
+      <c r="D7" s="1">
+        <v>10.57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3.74</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.64</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6.58</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6.48</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6.69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.29</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1">
+        <v>36.35</v>
+      </c>
+      <c r="C11" s="1">
+        <v>35.83</v>
+      </c>
+      <c r="D11" s="1">
+        <v>36.869999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3.64</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3.55</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1">
+        <v>32.74</v>
+      </c>
+      <c r="C13" s="1">
+        <v>32.25</v>
+      </c>
+      <c r="D13" s="1">
+        <v>33.24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6.18</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6.61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1">
+        <v>6.37</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6.24</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6.51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4.18</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>109.8719</v>
+      </c>
+      <c r="C17" s="1">
+        <v>108.2811</v>
+      </c>
+      <c r="D17" s="1">
+        <v>111.47239999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1">
+        <v>6.15</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5.91</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6.39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2.94</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2.77</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2.12</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.36</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.61</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1.56</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="1">
+        <v>7.42</v>
+      </c>
+      <c r="C25" s="1">
+        <v>7.15</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4.34</v>
+      </c>
+      <c r="C26" s="1">
+        <v>4.22</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4.46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3.31</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1">
+        <v>20.91</v>
+      </c>
+      <c r="C28" s="1">
+        <v>20.51</v>
+      </c>
+      <c r="D28" s="1">
+        <v>21.32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6.53</v>
+      </c>
+      <c r="C29" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="D29" s="1">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="1">
+        <v>32.326799999999999</v>
+      </c>
+      <c r="C30" s="1">
+        <v>31.527000000000001</v>
+      </c>
+      <c r="D30" s="1">
+        <v>33.126599999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2.67</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2.59</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4.66</v>
+      </c>
+      <c r="C32" s="1">
+        <v>4.51</v>
+      </c>
+      <c r="D32" s="1">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="1">
+        <v>94.76</v>
+      </c>
+      <c r="C33" s="1">
+        <v>93.54</v>
+      </c>
+      <c r="D33" s="1">
+        <v>95.97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="1">
+        <v>9.06</v>
+      </c>
+      <c r="C34" s="1">
+        <v>8.89</v>
+      </c>
+      <c r="D34" s="1">
+        <v>9.23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2.84</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2.81</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="1">
+        <v>8.08</v>
+      </c>
+      <c r="C36" s="1">
+        <v>7.86</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8.31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="1">
+        <v>68.69</v>
+      </c>
+      <c r="C37" s="1">
+        <v>67.62</v>
+      </c>
+      <c r="D37" s="1">
+        <v>69.77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="1">
+        <v>5.67</v>
+      </c>
+      <c r="C38" s="1">
+        <v>5.52</v>
+      </c>
+      <c r="D38" s="1">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="1">
+        <v>4.37</v>
+      </c>
+      <c r="C39" s="1">
+        <v>4.24</v>
+      </c>
+      <c r="D39" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="11">
+        <v>74.69</v>
+      </c>
+      <c r="C40" s="11">
+        <v>69.66</v>
+      </c>
+      <c r="D40" s="11">
+        <v>79.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>